<commit_message>
"does the specialization area mentioned.py" කියන, අලුත් Criteria එකක් Add කලා.
</commit_message>
<xml_diff>
--- a/Job Recomandation Criteria.xlsx
+++ b/Job Recomandation Criteria.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vikasitha\Documents\RP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECDA766F-F8D3-41C2-B94A-A9712A13B5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A19D75E-C3CA-4FD4-9B05-67951C68AAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,12 +28,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name of criteria</t>
   </si>
   <si>
     <t>Github Links Mention කරලා තියෙනවද / Github Links වැඩ කරනවද?</t>
+  </si>
+  <si>
+    <t>Degree name එක හරියට Mention කරලා තියෙනවද?</t>
+  </si>
+  <si>
+    <t>Specialization area එක Mention කරලා ද?</t>
+  </si>
+  <si>
+    <t>Add current GPA, if you have good results</t>
+  </si>
+  <si>
+    <t>(Bachelor of Information and Communication Technology (Hons))</t>
+  </si>
+  <si>
+    <t>(Software Technology/Network Technology/Multimedia Technology)</t>
+  </si>
+  <si>
+    <t>CV එකේ Pages එකකට වඩා තිබීම</t>
   </si>
 </sst>
 </file>
@@ -351,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -369,6 +387,36 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>